<commit_message>
Correcoes Tela / Adicionamento de Dependências
</commit_message>
<xml_diff>
--- a/excel/Arquivo.xlsx
+++ b/excel/Arquivo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Torneio</t>
   </si>
@@ -24,20 +24,14 @@
     <t>Rede</t>
   </si>
   <si>
-    <t>rede1</t>
-  </si>
-  <si>
-    <t>rede2</t>
-  </si>
-  <si>
-    <t>rede3</t>
+    <t>pokerstars</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,17 +48,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF3F7F5F"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
       <u/>
-      <sz val="10"/>
-      <color rgb="FF3F7F5F"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,15 +76,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,19 +381,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,30 +400,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3540607900</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3540607900</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
+      <c r="E3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Novas implementacoes e implantacao leitura arquivo Excel
</commit_message>
<xml_diff>
--- a/excel/Arquivo.xlsx
+++ b/excel/Arquivo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Torneio</t>
   </si>
@@ -25,6 +25,12 @@
   </si>
   <si>
     <t>pokerstars</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -381,18 +387,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E801"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -400,22 +407,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A401">
         <v>3540607900</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B401" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="C401">
+        <v>8358</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A402">
         <v>3540607900</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B402" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="C402">
+        <v>16712</v>
+      </c>
+      <c r="D402">
+        <v>8354</v>
+      </c>
+      <c r="E402">
+        <v>8358</v>
+      </c>
+    </row>
+    <row r="801" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A801">
+        <v>3540607900</v>
+      </c>
+      <c r="B801" t="s">
+        <v>2</v>
+      </c>
+      <c r="C801">
+        <v>8358</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correcoes formatacoes, erros de análise regex
</commit_message>
<xml_diff>
--- a/excel/Arquivo.xlsx
+++ b/excel/Arquivo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="3">
   <si>
     <t>Torneio</t>
   </si>
@@ -26,17 +26,12 @@
   <si>
     <t>pokerstars</t>
   </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -82,9 +77,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -390,16 +386,16 @@
   <dimension ref="A1:E801"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,61 +403,79 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>3.5406079E9</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="C2" t="n" s="0">
+        <v>16712.0</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>8354.0</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>8358.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>3.5406079E9</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>16712.0</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>8354.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>8358.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A401">
+      <c r="A401" s="0">
         <v>3540607900</v>
       </c>
-      <c r="B401" t="s">
+      <c r="B401" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C401">
+      <c r="C401" s="0">
         <v>8358</v>
       </c>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A402">
+      <c r="A402" s="0">
         <v>3540607900</v>
       </c>
-      <c r="B402" t="s">
+      <c r="B402" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C402">
+      <c r="C402" s="0">
         <v>16712</v>
       </c>
-      <c r="D402">
+      <c r="D402" s="0">
         <v>8354</v>
       </c>
-      <c r="E402">
+      <c r="E402" s="0">
         <v>8358</v>
       </c>
     </row>
     <row r="801" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A801">
+      <c r="A801" s="0">
         <v>3540607900</v>
       </c>
-      <c r="B801" t="s">
+      <c r="B801" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C801">
+      <c r="C801" s="0">
         <v>8358</v>
       </c>
     </row>

</xml_diff>